<commit_message>
new android chrome support
</commit_message>
<xml_diff>
--- a/src/global/utils/file-utils/locators.xlsx
+++ b/src/global/utils/file-utils/locators.xlsx
@@ -1187,10 +1187,10 @@
         <v>css</v>
       </c>
       <c r="D3" t="str">
-        <v>svg path[d^="M12 2.25a.75.75"]</v>
+        <v/>
       </c>
       <c r="E3" t="str">
-        <v>{}</v>
+        <v/>
       </c>
       <c r="F3" t="str">
         <v>0_x000d_</v>

</xml_diff>